<commit_message>
changed stimulus duration to 5 s, skipping 3rd task instructions, added white background to instruction screens, changed instruction text color to black
</commit_message>
<xml_diff>
--- a/blocks_pilot.xlsx
+++ b/blocks_pilot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85B2BED-1DB6-4978-96D5-3D651A340653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7285D1-6DB9-4D83-8F97-ECF066B873CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -420,7 +420,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,7 +472,7 @@
         <v>5</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -501,7 +501,7 @@
         <v>5</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -530,7 +530,7 @@
         <v>5</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F4">
         <v>10</v>

</xml_diff>

<commit_message>
working on staircasing the stimulus duration
</commit_message>
<xml_diff>
--- a/blocks_pilot.xlsx
+++ b/blocks_pilot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7285D1-6DB9-4D83-8F97-ECF066B873CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E23824B-4660-4774-9F75-84279DEC23D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12585" yWindow="2610" windowWidth="15615" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,14 +419,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.7109375" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -466,19 +466,19 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
@@ -495,19 +495,19 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="F3">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G3">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="H3" t="s">
         <v>10</v>
@@ -524,19 +524,19 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="F4">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G4">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="H4" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
sound cue plays simultaneously with text stim, exp now waits until a key press before initiating inter-trial intervals
</commit_message>
<xml_diff>
--- a/blocks_pilot.xlsx
+++ b/blocks_pilot.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E23824B-4660-4774-9F75-84279DEC23D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD46A338-9DB2-46B3-AABC-7EB60D9B457F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12585" yWindow="2610" windowWidth="15615" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -420,16 +420,16 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +458,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -487,7 +487,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -516,7 +516,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -545,7 +545,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
full task and its instructions are added to the pilot study, staircase algorithm is completed has not yet implemented
</commit_message>
<xml_diff>
--- a/blocks_pilot.xlsx
+++ b/blocks_pilot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFA6DD8-6480-41BD-B7FE-B97A0168E6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D1F93D-0A26-4AB4-8331-3453BA1BF3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="2985" windowWidth="20295" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>current_font</t>
   </si>
@@ -100,6 +100,15 @@
   </si>
   <si>
     <t>wh_ratio</t>
+  </si>
+  <si>
+    <t>full_task_roboto</t>
+  </si>
+  <si>
+    <t>full_task_neuefrutigerworld</t>
+  </si>
+  <si>
+    <t>./instructions_pilot/full_task.png</t>
   </si>
 </sst>
 </file>
@@ -417,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,6 +598,70 @@
         <v>1.77</v>
       </c>
     </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>25</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7">
+        <v>1.77</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finish instruction now appears as it should
</commit_message>
<xml_diff>
--- a/blocks_pilot.xlsx
+++ b/blocks_pilot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D1F93D-0A26-4AB4-8331-3453BA1BF3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF665FF6-D77D-4768-BC14-0660C1EC14B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -429,7 +429,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
staircase implemented in the task, fonts are now displayed properly
</commit_message>
<xml_diff>
--- a/blocks_pilot.xlsx
+++ b/blocks_pilot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38531CC-0727-4D7A-AB02-E1950FC9316E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5715E2B-8856-4C9B-8A65-D048ACE8A57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>current_font</t>
   </si>
@@ -54,9 +54,6 @@
     <t>iti_max</t>
   </si>
   <si>
-    <t>stimulus_duration</t>
-  </si>
-  <si>
     <t>lexical_wo_driving_roboto</t>
   </si>
   <si>
@@ -72,15 +69,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>./fonts/georgia.ttf</t>
-  </si>
-  <si>
-    <t>./fonts/robotoflex.ttf</t>
-  </si>
-  <si>
-    <t>./fonts/neuefrutigerworld.ttf</t>
-  </si>
-  <si>
     <t>word_trial_count</t>
   </si>
   <si>
@@ -109,6 +97,15 @@
   </si>
   <si>
     <t>./instructions_pilot/full_task.png</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>RobotoFlex</t>
+  </si>
+  <si>
+    <t>Neue Frutiger World</t>
   </si>
 </sst>
 </file>
@@ -426,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,7 +435,7 @@
     <col min="2" max="2" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,63 +449,57 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0.5</v>
-      </c>
-      <c r="F2">
-        <v>20</v>
-      </c>
-      <c r="G2">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2">
-        <v>1.77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
       <c r="C3">
         <v>1</v>
       </c>
@@ -516,59 +507,53 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0.5</v>
+        <v>40</v>
       </c>
       <c r="F3">
         <v>40</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>40</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3">
-        <v>1.77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0.5</v>
       </c>
       <c r="F4">
         <v>40</v>
       </c>
-      <c r="G4">
-        <v>40</v>
+      <c r="G4" t="s">
+        <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4">
+        <v>14</v>
+      </c>
+      <c r="I4">
         <v>1.77</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -580,30 +565,27 @@
         <v>25</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
-      <c r="G5">
-        <v>4</v>
+      <c r="G5" t="s">
+        <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5">
+        <v>15</v>
+      </c>
+      <c r="I5">
         <v>1.77</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>15</v>
@@ -612,30 +594,27 @@
         <v>25</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F6">
         <v>6</v>
       </c>
-      <c r="G6">
-        <v>6</v>
+      <c r="G6" t="s">
+        <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6">
+        <v>20</v>
+      </c>
+      <c r="I6">
         <v>1.77</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>15</v>
@@ -644,21 +623,18 @@
         <v>25</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F7">
         <v>6</v>
       </c>
-      <c r="G7">
-        <v>6</v>
+      <c r="G7" t="s">
+        <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7">
+        <v>20</v>
+      </c>
+      <c r="I7">
         <v>1.77</v>
       </c>
     </row>

</xml_diff>

<commit_message>
stimulus size is in visual degrees now
</commit_message>
<xml_diff>
--- a/blocks_pilot.xlsx
+++ b/blocks_pilot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5715E2B-8856-4C9B-8A65-D048ACE8A57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3991DB-A7A2-44E5-92DF-88F1DB441A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>current_font</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Neue Frutiger World</t>
+  </si>
+  <si>
+    <t>xheight_to_size</t>
   </si>
 </sst>
 </file>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,7 +438,7 @@
     <col min="2" max="2" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,8 +466,11 @@
       <c r="I1" t="s">
         <v>17</v>
       </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -478,10 +484,10 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -492,8 +498,11 @@
       <c r="I2">
         <v>1.77</v>
       </c>
+      <c r="J2">
+        <v>2.0699999999999998</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -521,8 +530,11 @@
       <c r="I3">
         <v>1.77</v>
       </c>
+      <c r="J3">
+        <v>1.9824999999999999</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -550,8 +562,11 @@
       <c r="I4">
         <v>1.77</v>
       </c>
+      <c r="J4">
+        <v>1.96</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -579,8 +594,11 @@
       <c r="I5">
         <v>1.77</v>
       </c>
+      <c r="J5">
+        <v>2.0699999999999998</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -608,8 +626,11 @@
       <c r="I6">
         <v>1.77</v>
       </c>
+      <c r="J6">
+        <v>1.9824999999999999</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -636,6 +657,9 @@
       </c>
       <c r="I7">
         <v>1.77</v>
+      </c>
+      <c r="J7">
+        <v>1.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stimulus size changed, elapsed_time column added to the data sheet
</commit_message>
<xml_diff>
--- a/blocks_pilot.xlsx
+++ b/blocks_pilot.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3991DB-A7A2-44E5-92DF-88F1DB441A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A303020-AAD5-44E5-B1EE-E83A1FE06678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -429,7 +429,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed staircasing, added mask and sound cue
</commit_message>
<xml_diff>
--- a/blocks_pilot.xlsx
+++ b/blocks_pilot.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\repos\driving_sim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A303020-AAD5-44E5-B1EE-E83A1FE06678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E73CF6-F759-4689-B229-5C6F9C7577F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>current_font</t>
   </si>
@@ -63,52 +63,55 @@
     <t>enableSound</t>
   </si>
   <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>word_trial_count</t>
+  </si>
+  <si>
+    <t>nonword_trial_count</t>
+  </si>
+  <si>
+    <t>./instructions_pilot/lexical_training.png</t>
+  </si>
+  <si>
+    <t>./instructions_pilot/lexical_task.png</t>
+  </si>
+  <si>
+    <t>./instructions_pilot/driving_lexical_training.png</t>
+  </si>
+  <si>
+    <t>instruction_image_file</t>
+  </si>
+  <si>
+    <t>wh_ratio</t>
+  </si>
+  <si>
+    <t>full_task_roboto</t>
+  </si>
+  <si>
+    <t>full_task_neuefrutigerworld</t>
+  </si>
+  <si>
+    <t>./instructions_pilot/full_task.png</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>RobotoFlex</t>
+  </si>
+  <si>
+    <t>Neue Frutiger World</t>
+  </si>
+  <si>
+    <t>xheight_to_size</t>
+  </si>
+  <si>
+    <t>maskEnabled</t>
+  </si>
+  <si>
     <t>no</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>word_trial_count</t>
-  </si>
-  <si>
-    <t>nonword_trial_count</t>
-  </si>
-  <si>
-    <t>./instructions_pilot/lexical_training.png</t>
-  </si>
-  <si>
-    <t>./instructions_pilot/lexical_task.png</t>
-  </si>
-  <si>
-    <t>./instructions_pilot/driving_lexical_training.png</t>
-  </si>
-  <si>
-    <t>instruction_image_file</t>
-  </si>
-  <si>
-    <t>wh_ratio</t>
-  </si>
-  <si>
-    <t>full_task_roboto</t>
-  </si>
-  <si>
-    <t>full_task_neuefrutigerworld</t>
-  </si>
-  <si>
-    <t>./instructions_pilot/full_task.png</t>
-  </si>
-  <si>
-    <t>Georgia</t>
-  </si>
-  <si>
-    <t>RobotoFlex</t>
-  </si>
-  <si>
-    <t>Neue Frutiger World</t>
-  </si>
-  <si>
-    <t>xheight_to_size</t>
   </si>
 </sst>
 </file>
@@ -426,19 +429,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,27 +455,30 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
         <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
       </c>
       <c r="G1" t="s">
         <v>8</v>
       </c>
       <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
       <c r="J1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -493,7 +499,7 @@
         <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2">
         <v>1.77</v>
@@ -501,10 +507,13 @@
       <c r="J2">
         <v>2.0699999999999998</v>
       </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -516,16 +525,16 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F3">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3">
         <v>1.77</v>
@@ -533,10 +542,13 @@
       <c r="J3">
         <v>1.9824999999999999</v>
       </c>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -548,16 +560,16 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F4">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I4">
         <v>1.77</v>
@@ -565,10 +577,13 @@
       <c r="J4">
         <v>1.96</v>
       </c>
+      <c r="K4" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -586,10 +601,10 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I5">
         <v>1.77</v>
@@ -597,13 +612,16 @@
       <c r="J5">
         <v>2.0699999999999998</v>
       </c>
+      <c r="K5" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>15</v>
@@ -618,10 +636,10 @@
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6">
         <v>1.77</v>
@@ -629,13 +647,16 @@
       <c r="J6">
         <v>1.9824999999999999</v>
       </c>
+      <c r="K6" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>15</v>
@@ -650,16 +671,19 @@
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I7">
         <v>1.77</v>
       </c>
       <c r="J7">
         <v>1.96</v>
+      </c>
+      <c r="K7" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
increased practice trials from 2 to 40
</commit_message>
<xml_diff>
--- a/blocks_pilot.xlsx
+++ b/blocks_pilot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54DCC48-841B-441E-B320-3066A48FD561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B16A769-52A8-4BF0-9412-A39D21A197D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -432,7 +432,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,10 +490,10 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
fixed crash error, decreased ITI and increased trials during driving+lexical, increased training trials of lexical only training
</commit_message>
<xml_diff>
--- a/blocks_pilot.xlsx
+++ b/blocks_pilot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA388E96-4D7D-479E-B9B0-ECF718DBF712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB3F832-61A3-49FA-8B74-1667B1A63834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11895" yWindow="3765" windowWidth="12360" windowHeight="10950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -431,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,13 +490,13 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -531,7 +531,7 @@
         <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
@@ -566,7 +566,7 @@
         <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s">
         <v>13</v>
@@ -589,16 +589,16 @@
         <v>2</v>
       </c>
       <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
         <v>15</v>
       </c>
-      <c r="D5">
-        <v>25</v>
-      </c>
       <c r="E5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
@@ -624,16 +624,16 @@
         <v>17</v>
       </c>
       <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
         <v>15</v>
       </c>
-      <c r="D6">
-        <v>25</v>
-      </c>
       <c r="E6">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F6">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -659,16 +659,16 @@
         <v>18</v>
       </c>
       <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
         <v>15</v>
       </c>
-      <c r="D7">
-        <v>25</v>
-      </c>
       <c r="E7">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F7">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
added a score screen at the end of the experiment
</commit_message>
<xml_diff>
--- a/blocks_pilot.xlsx
+++ b/blocks_pilot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB3F832-61A3-49FA-8B74-1667B1A63834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3D63E2-903C-4AFE-ABCB-B8EF7AE6BA47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -432,7 +432,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
button press now terminates stimulus display, score screen updated for only driving+lexical, comission error added for presses during masks/fixation
</commit_message>
<xml_diff>
--- a/blocks_pilot.xlsx
+++ b/blocks_pilot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\All Files\Genel\Is\2022\Upwork\LabX\studies\materials\drivingSimulator\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3D63E2-903C-4AFE-ABCB-B8EF7AE6BA47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346BAA67-4042-43CD-AC18-98E4C49AF247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -432,7 +432,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>